<commit_message>
change layout master barang multi satuan
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterBarangMultiSatuan.xlsx
+++ b/ImportExport/ExcelFiles/MasterBarangMultiSatuan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\AXATA\AxataPOSFilesResources\AxataPOSFilesResources\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032EBD34-427F-40EF-9A4F-11FD37244401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E5F304-E4F6-4BC4-A6E6-077767139F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>NAMABARANG</t>
   </si>
@@ -44,27 +44,12 @@
     <t>MERKBARANG</t>
   </si>
   <si>
-    <t>SATUAN</t>
-  </si>
-  <si>
-    <t>HARGABELI</t>
-  </si>
-  <si>
-    <t>HARGAJUAL</t>
-  </si>
-  <si>
-    <t>BARCODE</t>
-  </si>
-  <si>
     <t>NAMASUPPLIER</t>
   </si>
   <si>
     <t>RAK</t>
   </si>
   <si>
-    <t>JMLBARANG</t>
-  </si>
-  <si>
     <t>ISI1</t>
   </si>
   <si>
@@ -135,6 +120,51 @@
   </si>
   <si>
     <t>SHGD24153W5</t>
+  </si>
+  <si>
+    <t>SATUAN1</t>
+  </si>
+  <si>
+    <t>HARGABELI1</t>
+  </si>
+  <si>
+    <t>HARGAJUAL1</t>
+  </si>
+  <si>
+    <t>JMLBARANG1</t>
+  </si>
+  <si>
+    <t>BARCODE1</t>
+  </si>
+  <si>
+    <t>SATUAN2</t>
+  </si>
+  <si>
+    <t>HARGABELI2</t>
+  </si>
+  <si>
+    <t>HARGAJUAL2</t>
+  </si>
+  <si>
+    <t>JMLBARANG2</t>
+  </si>
+  <si>
+    <t>BARCODE2</t>
+  </si>
+  <si>
+    <t>SATUAN3</t>
+  </si>
+  <si>
+    <t>HARGABELI3</t>
+  </si>
+  <si>
+    <t>HARGAJUAL3</t>
+  </si>
+  <si>
+    <t>JMLBARANG3</t>
+  </si>
+  <si>
+    <t>BARCODE3</t>
   </si>
 </sst>
 </file>
@@ -525,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -537,23 +567,23 @@
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -567,87 +597,87 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="S1" s="7" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="W1" s="7" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H2" s="4">
         <v>2000</v>
@@ -659,13 +689,13 @@
         <v>5</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L2" s="6">
         <v>1</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="N2" s="6">
         <v>2000</v>
@@ -677,7 +707,7 @@
         <v>5</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="R2" s="8">
         <v>0</v>
@@ -690,25 +720,25 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H3" s="4">
         <v>2000</v>
@@ -720,13 +750,13 @@
         <v>5</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L3" s="6">
         <v>1</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="N3" s="6">
         <v>2000</v>
@@ -738,7 +768,7 @@
         <v>5</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="R3" s="8">
         <v>0</v>
@@ -751,25 +781,25 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H4" s="4">
         <v>2000</v>
@@ -781,13 +811,13 @@
         <v>5</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L4" s="6">
         <v>1</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="N4" s="6">
         <v>2000</v>
@@ -799,7 +829,7 @@
         <v>5</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="R4" s="8">
         <v>0</v>
@@ -812,25 +842,25 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H5" s="4">
         <v>200</v>
@@ -842,13 +872,13 @@
         <v>5</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L5" s="6">
         <v>1</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="N5" s="6">
         <v>200</v>
@@ -860,7 +890,7 @@
         <v>5</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="R5" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
update layout master barang multi satuan
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterBarangMultiSatuan.xlsx
+++ b/ImportExport/ExcelFiles/MasterBarangMultiSatuan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\AXATA\AxataPOSFilesResources\AxataPOSFilesResources\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E5F304-E4F6-4BC4-A6E6-077767139F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5419950D-492B-4F84-8CDA-2FB8D918D991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>NAMABARANG</t>
   </si>
@@ -131,9 +131,6 @@
     <t>HARGAJUAL1</t>
   </si>
   <si>
-    <t>JMLBARANG1</t>
-  </si>
-  <si>
     <t>BARCODE1</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>HARGAJUAL2</t>
   </si>
   <si>
-    <t>JMLBARANG2</t>
-  </si>
-  <si>
     <t>BARCODE2</t>
   </si>
   <si>
@@ -161,10 +155,10 @@
     <t>HARGAJUAL3</t>
   </si>
   <si>
-    <t>JMLBARANG3</t>
-  </si>
-  <si>
     <t>BARCODE3</t>
+  </si>
+  <si>
+    <t>JMLSTOK</t>
   </si>
 </sst>
 </file>
@@ -250,7 +244,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -276,6 +270,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -553,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -566,27 +563,25 @@
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -602,62 +597,56 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>43</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -673,20 +662,20 @@
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="9">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="4">
+      <c r="I2" s="4">
         <v>2000</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="4">
         <v>3000</v>
-      </c>
-      <c r="J2" s="4">
-        <v>5</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>23</v>
@@ -703,22 +692,18 @@
       <c r="O2" s="6">
         <v>3000</v>
       </c>
-      <c r="P2" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="8">
+      <c r="Q2" s="8">
         <v>0</v>
       </c>
+      <c r="R2" s="8"/>
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -734,20 +719,20 @@
       <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="9">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>2000</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>3000</v>
-      </c>
-      <c r="J3" s="4">
-        <v>5</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>23</v>
@@ -764,22 +749,18 @@
       <c r="O3" s="6">
         <v>3000</v>
       </c>
-      <c r="P3" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="8">
+      <c r="Q3" s="8">
         <v>0</v>
       </c>
+      <c r="R3" s="8"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -795,20 +776,20 @@
       <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="9">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>2000</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>3000</v>
-      </c>
-      <c r="J4" s="4">
-        <v>5</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>23</v>
@@ -825,22 +806,18 @@
       <c r="O4" s="6">
         <v>3000</v>
       </c>
-      <c r="P4" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="8">
+      <c r="Q4" s="8">
         <v>0</v>
       </c>
+      <c r="R4" s="8"/>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
       <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -856,20 +833,20 @@
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="9">
+        <v>5</v>
+      </c>
+      <c r="G5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>200</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="4">
         <v>3000</v>
-      </c>
-      <c r="J5" s="4">
-        <v>5</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>23</v>
@@ -886,20 +863,16 @@
       <c r="O5" s="6">
         <v>3000</v>
       </c>
-      <c r="P5" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="8">
+      <c r="Q5" s="8">
         <v>0</v>
       </c>
+      <c r="R5" s="8"/>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
update layout master barang multi satuan dan Tambah master barang pelanggan
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterBarangMultiSatuan.xlsx
+++ b/ImportExport/ExcelFiles/MasterBarangMultiSatuan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\AXATA\AxataPOSFilesResources\AxataPOSFilesResources\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F652C480-809C-484A-9C9D-7839AE91E97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A41E18-E8AF-4145-B1EC-667E3BEA5050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -544,7 +544,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -670,7 +670,7 @@
         <v>22</v>
       </c>
       <c r="N2" s="6">
-        <v>3000</v>
+        <v>19000</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>23</v>
@@ -723,7 +723,7 @@
         <v>22</v>
       </c>
       <c r="N3" s="6">
-        <v>3000</v>
+        <v>19000</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>24</v>
@@ -776,7 +776,7 @@
         <v>22</v>
       </c>
       <c r="N4" s="6">
-        <v>3000</v>
+        <v>19000</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>25</v>
@@ -808,7 +808,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="1">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="H5" s="4">
         <v>1</v>
@@ -829,7 +829,7 @@
         <v>22</v>
       </c>
       <c r="N5" s="6">
-        <v>3000</v>
+        <v>19000</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
update master barang multi satuan
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterBarangMultiSatuan.xlsx
+++ b/ImportExport/ExcelFiles/MasterBarangMultiSatuan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\AXATA\AxataPOSFilesResources\AxataPOSFilesResources\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B7C1BE-A398-4F7A-A4F9-63BFC90131BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1572CF67-1979-48F0-BC72-A228FB630A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>NAMABARANG</t>
   </si>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -756,9 +756,7 @@
       <c r="J3" s="4">
         <v>3000</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="K3" s="4"/>
       <c r="L3" s="6">
         <v>0</v>
       </c>
@@ -809,9 +807,7 @@
       <c r="J4" s="4">
         <v>3000</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="K4" s="4"/>
       <c r="L4" s="6">
         <v>10</v>
       </c>
@@ -868,9 +864,7 @@
       <c r="J5" s="4">
         <v>3000</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="K5" s="4"/>
       <c r="L5" s="6">
         <v>10</v>
       </c>

</xml_diff>